<commit_message>
1. Added Loan Unit Tests 2. Added namespaces 3. Code cleanup 4. Added composite calendar
</commit_message>
<xml_diff>
--- a/Documentation/LoanCalculator.xlsx
+++ b/Documentation/LoanCalculator.xlsx
@@ -1,24 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramiz\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -136,13 +131,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;₽&quot;"/>
-    <numFmt numFmtId="166" formatCode="yyyymmdd"/>
-    <numFmt numFmtId="167" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="yyyymmdd"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,13 +183,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Процентный" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -211,21 +206,9 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:lang val="ru-RU"/>
   <c:chart>
     <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -254,12 +237,10 @@
         </a:p>
       </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -291,7 +272,7 @@
             <c:numRef>
               <c:f>Sheet1!$D$7:$D$28</c:f>
               <c:numCache>
-                <c:formatCode>#\ ##0.00\ "₽"</c:formatCode>
+                <c:formatCode>#,##0.00\ "₽"</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
@@ -362,25 +343,16 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="262245136"/>
-        <c:axId val="262246224"/>
+        <c:dLbls/>
+        <c:axId val="110546944"/>
+        <c:axId val="110548480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="262245136"/>
+        <c:axId val="110546944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -397,7 +369,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -432,16 +403,15 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="262246224"/>
+        <c:crossAx val="110548480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="262246224"/>
+        <c:axId val="110548480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -457,9 +427,8 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="#\ ##0.00\ &quot;₽&quot;" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00\ &quot;₽&quot;" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -494,7 +463,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="262245136"/>
+        <c:crossAx val="110546944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -508,7 +477,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -537,7 +505,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1177,7 +1145,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1212,7 +1180,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1389,21 +1357,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
@@ -1412,7 +1380,7 @@
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1427,7 +1395,7 @@
         <v>124000</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1442,7 +1410,7 @@
         <v>5166.666666666667</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1451,7 +1419,7 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1468,7 +1436,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>0</v>
       </c>
@@ -1489,7 +1457,7 @@
         <v>4166.666666666667</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1518,7 +1486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1551,7 +1519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1584,7 +1552,7 @@
         <v>2.0100000000006766</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1617,7 +1585,7 @@
         <v>3.0301000000009588</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>5</v>
       </c>
@@ -1650,7 +1618,7 @@
         <v>4.0604010000012059</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1683,7 +1651,7 @@
         <v>5.1010050100017361</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1716,7 +1684,7 @@
         <v>6.1520150601020402</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>8</v>
       </c>
@@ -1749,7 +1717,7 @@
         <v>7.213535210703399</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>9</v>
       </c>
@@ -1782,7 +1750,7 @@
         <v>8.2856705628108234</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>10</v>
       </c>
@@ -1815,7 +1783,7 @@
         <v>9.3685272684394914</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>11</v>
       </c>
@@ -1848,7 +1816,7 @@
         <v>10.46221254112405</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>12</v>
       </c>
@@ -1881,7 +1849,7 @@
         <v>11.566834666535694</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20">
         <v>13</v>
       </c>
@@ -1914,7 +1882,7 @@
         <v>12.682503013201424</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21">
         <v>14</v>
       </c>
@@ -1947,7 +1915,7 @@
         <v>13.809328043333812</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22">
         <v>15</v>
       </c>
@@ -1980,7 +1948,7 @@
         <v>14.947421323767575</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23">
         <v>16</v>
       </c>
@@ -2013,7 +1981,7 @@
         <v>16.096895537005448</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24">
         <v>17</v>
       </c>
@@ -2046,7 +2014,7 @@
         <v>17.257864492376033</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25">
         <v>18</v>
       </c>
@@ -2079,7 +2047,7 @@
         <v>18.43044313730006</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26">
         <v>19</v>
       </c>
@@ -2112,7 +2080,7 @@
         <v>19.614747568673483</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27">
         <v>20</v>
       </c>
@@ -2145,7 +2113,7 @@
         <v>20.810895044360574</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28">
         <v>21</v>
       </c>
@@ -2178,7 +2146,7 @@
         <v>22.019003994804503</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29">
         <v>22</v>
       </c>
@@ -2186,7 +2154,7 @@
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30">
         <v>23</v>
       </c>
@@ -2194,7 +2162,7 @@
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="C31" s="1">
         <f>SUM(C7:C28)</f>
         <v>111701.72510378294</v>
@@ -2215,18 +2183,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="B141" sqref="B141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
@@ -2239,7 +2207,7 @@
     <col min="20" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2289,7 +2257,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -2337,7 +2305,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2385,7 +2353,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -2436,7 +2404,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2485,7 +2453,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20">
       <c r="G6" s="4">
         <f t="shared" si="0"/>
         <v>0.05</v>
@@ -2527,7 +2495,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2576,7 +2544,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20">
       <c r="G8" s="4">
         <f t="shared" si="0"/>
         <v>7.0000000000000007E-2</v>
@@ -2618,7 +2586,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2667,7 +2635,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2716,7 +2684,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20">
       <c r="G11" s="4">
         <f t="shared" si="0"/>
         <v>0.1</v>
@@ -2758,7 +2726,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20">
       <c r="G12" s="4">
         <f t="shared" si="0"/>
         <v>0.10999999999999999</v>
@@ -2800,7 +2768,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20">
       <c r="G13" s="4">
         <f t="shared" si="0"/>
         <v>0.12</v>
@@ -2854,7 +2822,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -2900,7 +2868,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20">
       <c r="A15">
         <v>0</v>
       </c>
@@ -2937,7 +2905,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20">
       <c r="A16">
         <v>1</v>
       </c>
@@ -2986,7 +2954,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20">
       <c r="A17">
         <v>2</v>
       </c>
@@ -3035,7 +3003,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20">
       <c r="A18">
         <v>3</v>
       </c>
@@ -3084,7 +3052,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20">
       <c r="A19">
         <v>4</v>
       </c>
@@ -3130,7 +3098,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20">
       <c r="A20">
         <v>5</v>
       </c>
@@ -3176,7 +3144,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20">
       <c r="A21">
         <v>6</v>
       </c>
@@ -3222,7 +3190,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20">
       <c r="A22">
         <v>7</v>
       </c>
@@ -3268,7 +3236,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20">
       <c r="A23">
         <v>8</v>
       </c>
@@ -3314,7 +3282,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20">
       <c r="A24">
         <v>9</v>
       </c>
@@ -3360,7 +3328,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20">
       <c r="A25">
         <v>10</v>
       </c>
@@ -3414,7 +3382,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20">
       <c r="A26">
         <v>11</v>
       </c>
@@ -3443,7 +3411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20">
       <c r="A27">
         <v>12</v>
       </c>
@@ -3472,7 +3440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20">
       <c r="A28">
         <v>13</v>
       </c>
@@ -3501,7 +3469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20">
       <c r="A29">
         <v>14</v>
       </c>
@@ -3530,7 +3498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20">
       <c r="A30">
         <v>15</v>
       </c>
@@ -3559,7 +3527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20">
       <c r="A31">
         <v>16</v>
       </c>
@@ -3588,7 +3556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20">
       <c r="A32">
         <v>17</v>
       </c>
@@ -3617,7 +3585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17">
       <c r="A33">
         <v>18</v>
       </c>
@@ -3646,7 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17">
       <c r="A34">
         <v>19</v>
       </c>
@@ -3675,7 +3643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17">
       <c r="A35">
         <v>20</v>
       </c>
@@ -3704,7 +3672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17">
       <c r="A36">
         <v>21</v>
       </c>
@@ -3733,7 +3701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17">
       <c r="A37">
         <v>22</v>
       </c>
@@ -3762,7 +3730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17">
       <c r="A38">
         <v>23</v>
       </c>
@@ -3791,7 +3759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17">
       <c r="A39">
         <v>24</v>
       </c>
@@ -3821,7 +3789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17">
       <c r="A40">
         <v>25</v>
       </c>
@@ -3850,7 +3818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17">
       <c r="A41">
         <v>26</v>
       </c>
@@ -3879,7 +3847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17">
       <c r="A42">
         <v>27</v>
       </c>
@@ -3908,7 +3876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17">
       <c r="A43">
         <v>28</v>
       </c>
@@ -3937,7 +3905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17">
       <c r="A44">
         <v>29</v>
       </c>
@@ -3966,7 +3934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17">
       <c r="A45">
         <v>30</v>
       </c>
@@ -3995,7 +3963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17">
       <c r="A46">
         <v>31</v>
       </c>
@@ -4024,7 +3992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17">
       <c r="A47">
         <v>32</v>
       </c>
@@ -4053,7 +4021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17">
       <c r="A48">
         <v>33</v>
       </c>
@@ -4082,7 +4050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17">
       <c r="A49">
         <v>34</v>
       </c>
@@ -4111,7 +4079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17">
       <c r="A50">
         <v>35</v>
       </c>
@@ -4140,7 +4108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17">
       <c r="A51">
         <v>36</v>
       </c>
@@ -4169,7 +4137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17">
       <c r="A52">
         <v>37</v>
       </c>
@@ -4198,7 +4166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17">
       <c r="A53">
         <v>38</v>
       </c>
@@ -4227,7 +4195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17">
       <c r="A54">
         <v>39</v>
       </c>
@@ -4256,7 +4224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17">
       <c r="A55">
         <v>40</v>
       </c>
@@ -4285,7 +4253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17">
       <c r="A56">
         <v>41</v>
       </c>
@@ -4314,7 +4282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17">
       <c r="A57">
         <v>42</v>
       </c>
@@ -4343,7 +4311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17">
       <c r="A58">
         <v>43</v>
       </c>
@@ -4372,7 +4340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17">
       <c r="A59">
         <v>44</v>
       </c>
@@ -4401,7 +4369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17">
       <c r="A60">
         <v>45</v>
       </c>
@@ -4430,7 +4398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17">
       <c r="A61">
         <v>46</v>
       </c>
@@ -4459,7 +4427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17">
       <c r="A62">
         <v>47</v>
       </c>
@@ -4488,7 +4456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17">
       <c r="A63">
         <v>48</v>
       </c>
@@ -4517,7 +4485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17">
       <c r="A64">
         <v>49</v>
       </c>
@@ -4546,7 +4514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17">
       <c r="A65">
         <v>50</v>
       </c>
@@ -4575,7 +4543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17">
       <c r="A66">
         <v>51</v>
       </c>
@@ -4604,7 +4572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17">
       <c r="A67">
         <v>52</v>
       </c>
@@ -4633,7 +4601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17">
       <c r="A68">
         <v>53</v>
       </c>
@@ -4662,7 +4630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17">
       <c r="A69">
         <v>54</v>
       </c>
@@ -4691,7 +4659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17">
       <c r="A70">
         <v>55</v>
       </c>
@@ -4720,7 +4688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17">
       <c r="A71">
         <v>56</v>
       </c>
@@ -4749,7 +4717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17">
       <c r="A72">
         <v>57</v>
       </c>
@@ -4778,7 +4746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17">
       <c r="A73">
         <v>58</v>
       </c>
@@ -4807,7 +4775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17">
       <c r="A74">
         <v>59</v>
       </c>
@@ -4836,7 +4804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17">
       <c r="A75">
         <v>60</v>
       </c>
@@ -4865,7 +4833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17">
       <c r="A76">
         <v>61</v>
       </c>
@@ -4894,7 +4862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17">
       <c r="A77">
         <v>62</v>
       </c>
@@ -4923,7 +4891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17">
       <c r="A78">
         <v>63</v>
       </c>
@@ -4952,7 +4920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17">
       <c r="A79">
         <v>64</v>
       </c>
@@ -4981,7 +4949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17">
       <c r="A80">
         <v>65</v>
       </c>
@@ -5010,7 +4978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17">
       <c r="A81">
         <v>66</v>
       </c>
@@ -5039,7 +5007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17">
       <c r="A82">
         <v>67</v>
       </c>
@@ -5068,7 +5036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17">
       <c r="A83">
         <v>68</v>
       </c>
@@ -5097,7 +5065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17">
       <c r="A84">
         <v>69</v>
       </c>
@@ -5126,7 +5094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17">
       <c r="A85">
         <v>70</v>
       </c>
@@ -5155,7 +5123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17">
       <c r="A86">
         <v>71</v>
       </c>
@@ -5184,7 +5152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17">
       <c r="A87">
         <v>72</v>
       </c>
@@ -5213,7 +5181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17">
       <c r="A88">
         <v>73</v>
       </c>
@@ -5242,7 +5210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17">
       <c r="A89">
         <v>74</v>
       </c>
@@ -5271,7 +5239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17">
       <c r="A90">
         <v>75</v>
       </c>
@@ -5300,7 +5268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17">
       <c r="A91">
         <v>76</v>
       </c>
@@ -5329,7 +5297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17">
       <c r="A92">
         <v>77</v>
       </c>
@@ -5358,7 +5326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17">
       <c r="A93">
         <v>78</v>
       </c>
@@ -5387,7 +5355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17">
       <c r="A94">
         <v>79</v>
       </c>
@@ -5416,7 +5384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17">
       <c r="A95">
         <v>80</v>
       </c>
@@ -5445,7 +5413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17">
       <c r="A96">
         <v>81</v>
       </c>
@@ -5474,7 +5442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17">
       <c r="A97">
         <v>82</v>
       </c>
@@ -5503,7 +5471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17">
       <c r="A98">
         <v>83</v>
       </c>
@@ -5532,7 +5500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17">
       <c r="A99">
         <v>84</v>
       </c>
@@ -5561,7 +5529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17">
       <c r="A100">
         <v>85</v>
       </c>
@@ -5590,7 +5558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17">
       <c r="A101">
         <v>86</v>
       </c>
@@ -5619,7 +5587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17">
       <c r="A102">
         <v>87</v>
       </c>
@@ -5648,7 +5616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17">
       <c r="A103">
         <v>88</v>
       </c>
@@ -5677,7 +5645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17">
       <c r="A104">
         <v>89</v>
       </c>
@@ -5706,7 +5674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17">
       <c r="A105">
         <v>90</v>
       </c>
@@ -5735,7 +5703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17">
       <c r="A106">
         <v>91</v>
       </c>
@@ -5764,7 +5732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17">
       <c r="A107">
         <v>92</v>
       </c>
@@ -5793,7 +5761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17">
       <c r="A108">
         <v>93</v>
       </c>
@@ -5822,7 +5790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17">
       <c r="A109">
         <v>94</v>
       </c>
@@ -5851,7 +5819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17">
       <c r="A110">
         <v>95</v>
       </c>
@@ -5880,7 +5848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17">
       <c r="A111">
         <v>96</v>
       </c>
@@ -5909,7 +5877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17">
       <c r="A112">
         <v>97</v>
       </c>
@@ -5938,7 +5906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17">
       <c r="A113">
         <v>98</v>
       </c>
@@ -5967,7 +5935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17">
       <c r="A114">
         <v>99</v>
       </c>
@@ -5996,7 +5964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17">
       <c r="A115">
         <v>100</v>
       </c>
@@ -6025,7 +5993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17">
       <c r="A116">
         <v>101</v>
       </c>
@@ -6054,7 +6022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17">
       <c r="A117">
         <v>102</v>
       </c>
@@ -6083,7 +6051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17">
       <c r="A118">
         <v>103</v>
       </c>
@@ -6112,7 +6080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17">
       <c r="A119">
         <v>104</v>
       </c>
@@ -6141,7 +6109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17">
       <c r="A120">
         <v>105</v>
       </c>
@@ -6170,7 +6138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:17">
       <c r="A121">
         <v>106</v>
       </c>
@@ -6199,7 +6167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:17">
       <c r="A122">
         <v>107</v>
       </c>
@@ -6228,7 +6196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:17">
       <c r="A123">
         <v>108</v>
       </c>
@@ -6257,7 +6225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:17">
       <c r="A124">
         <v>109</v>
       </c>
@@ -6286,7 +6254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:17">
       <c r="A125">
         <v>110</v>
       </c>
@@ -6315,7 +6283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:17">
       <c r="A126">
         <v>111</v>
       </c>
@@ -6344,7 +6312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:17">
       <c r="A127">
         <v>112</v>
       </c>
@@ -6373,7 +6341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17">
       <c r="A128">
         <v>113</v>
       </c>
@@ -6402,7 +6370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:17">
       <c r="A129">
         <v>114</v>
       </c>
@@ -6431,7 +6399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:17">
       <c r="A130">
         <v>115</v>
       </c>
@@ -6460,7 +6428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:17">
       <c r="A131">
         <v>116</v>
       </c>
@@ -6489,7 +6457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:17">
       <c r="A132">
         <v>117</v>
       </c>
@@ -6518,7 +6486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:17">
       <c r="A133">
         <v>118</v>
       </c>
@@ -6547,7 +6515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:17">
       <c r="A134">
         <v>119</v>
       </c>
@@ -6576,7 +6544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:17">
       <c r="A135">
         <v>120</v>
       </c>
@@ -6605,7 +6573,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:17">
+      <c r="C136" s="1">
+        <f>SUM(C16:C135)</f>
+        <v>6542275.2471580002</v>
+      </c>
+      <c r="D136" s="1">
+        <f>SUM(D16:D135)</f>
+        <v>2742275.2471579858</v>
+      </c>
+      <c r="E136" s="1">
+        <f>SUM(E16:E135)</f>
+        <v>3799999.9999999953</v>
+      </c>
       <c r="N136" s="8">
         <v>45717</v>
       </c>
@@ -6621,16 +6601,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -6638,17 +6618,17 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="B6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="B7" s="6">
         <v>42005</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="B8" s="6">
         <f>B7</f>
         <v>42005</v>

</xml_diff>